<commit_message>
Some slight changes to the Robotron 2084 sprites and added the ply model maker thingy
</commit_message>
<xml_diff>
--- a/6044_FramPat/SAM/Robotron 2084/Sprite map/sprite - Brain.xlsx
+++ b/6044_FramPat/SAM/Robotron 2084/Sprite map/sprite - Brain.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097F38C4-1F2F-4C7B-91CC-04191A1E2657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2526" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2526" uniqueCount="20">
   <si>
     <t>B</t>
   </si>
@@ -74,12 +75,15 @@
   <si>
     <t>Green</t>
   </si>
+  <si>
+    <t>g</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +243,14 @@
       <color rgb="FFFF66CC"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -259,7 +271,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPr id="1028" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -299,7 +317,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 6"/>
+        <xdr:cNvPr id="2" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -339,7 +363,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 8"/>
+        <xdr:cNvPr id="3" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -379,7 +409,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 10"/>
+        <xdr:cNvPr id="4" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -419,7 +455,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 12"/>
+        <xdr:cNvPr id="5" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -459,7 +501,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 14"/>
+        <xdr:cNvPr id="6" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -499,7 +547,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 16"/>
+        <xdr:cNvPr id="7" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -539,7 +593,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 18"/>
+        <xdr:cNvPr id="8" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -579,7 +639,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 20"/>
+        <xdr:cNvPr id="9" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -619,7 +685,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 22"/>
+        <xdr:cNvPr id="10" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -659,7 +731,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 24"/>
+        <xdr:cNvPr id="11" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -699,7 +777,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 26"/>
+        <xdr:cNvPr id="12" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -728,9 +812,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -768,7 +852,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -802,6 +886,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -836,9 +921,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1011,19 +1097,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CL74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="BS30" sqref="BS30"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="CL8" sqref="CL8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="98" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88">
+    <row r="1" spans="1:88" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -1142,7 +1228,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:88">
+    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1276,7 +1362,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:88">
+    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1410,7 +1496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:88">
+    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1544,7 +1630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:88">
+    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1678,7 +1764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:88">
+    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1812,7 +1898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:88">
+    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1946,7 +2032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:88">
+    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2074,13 +2160,13 @@
         <v>2</v>
       </c>
       <c r="CH8" s="8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="CJ8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:88">
+    <row r="9" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2214,7 +2300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:88">
+    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2348,7 +2434,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:88">
+    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2482,7 +2568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:88">
+    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2610,7 +2696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:88">
+    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2738,7 +2824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:88">
+    <row r="14" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2866,7 +2952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:88">
+    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2994,7 +3080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:88">
+    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3122,7 +3208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:90">
+    <row r="17" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3250,7 +3336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:90">
+    <row r="20" spans="1:90" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>0</v>
       </c>
@@ -3374,7 +3460,7 @@
       <c r="CK20" s="1"/>
       <c r="CL20" s="1"/>
     </row>
-    <row r="21" spans="1:90">
+    <row r="21" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -3502,7 +3588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:90">
+    <row r="22" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3630,7 +3716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:90">
+    <row r="23" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -3758,7 +3844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:90">
+    <row r="24" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3886,7 +3972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:90">
+    <row r="25" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -4014,7 +4100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:90">
+    <row r="26" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -4142,7 +4228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:90">
+    <row r="27" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6</v>
       </c>
@@ -4270,7 +4356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:90">
+    <row r="28" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -4398,7 +4484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:90">
+    <row r="29" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>8</v>
       </c>
@@ -4529,7 +4615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:90">
+    <row r="30" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>9</v>
       </c>
@@ -4660,7 +4746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:90">
+    <row r="31" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
@@ -4791,7 +4877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:90">
+    <row r="32" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>11</v>
       </c>
@@ -4922,7 +5008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:72">
+    <row r="33" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>12</v>
       </c>
@@ -5053,7 +5139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:72">
+    <row r="34" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>13</v>
       </c>
@@ -5184,7 +5270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:72">
+    <row r="35" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>14</v>
       </c>
@@ -5315,7 +5401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:72">
+    <row r="36" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15</v>
       </c>
@@ -5446,17 +5532,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:72">
+    <row r="37" spans="1:72" x14ac:dyDescent="0.25">
       <c r="AB37" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:72">
+    <row r="38" spans="1:72" x14ac:dyDescent="0.25">
       <c r="AB38" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:72">
+    <row r="39" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>0</v>
       </c>
@@ -5575,7 +5661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:72">
+    <row r="40" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0</v>
       </c>
@@ -5708,7 +5794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:72">
+    <row r="41" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -5841,7 +5927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:72">
+    <row r="42" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -5974,7 +6060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:72">
+    <row r="43" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -6107,7 +6193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:72">
+    <row r="44" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4</v>
       </c>
@@ -6240,7 +6326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:72">
+    <row r="45" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5</v>
       </c>
@@ -6373,7 +6459,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:72">
+    <row r="46" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6</v>
       </c>
@@ -6506,7 +6592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:72">
+    <row r="47" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7</v>
       </c>
@@ -6639,7 +6725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:72">
+    <row r="48" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>8</v>
       </c>
@@ -6772,7 +6858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:85">
+    <row r="49" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9</v>
       </c>
@@ -6905,7 +6991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:85">
+    <row r="50" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>10</v>
       </c>
@@ -7068,7 +7154,7 @@
       <c r="CF50" s="1"/>
       <c r="CG50" s="1"/>
     </row>
-    <row r="51" spans="1:85">
+    <row r="51" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>11</v>
       </c>
@@ -7200,7 +7286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:85">
+    <row r="52" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>12</v>
       </c>
@@ -7332,7 +7418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:85">
+    <row r="53" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>13</v>
       </c>
@@ -7464,7 +7550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:85">
+    <row r="54" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>14</v>
       </c>
@@ -7596,7 +7682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:85">
+    <row r="55" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>15</v>
       </c>
@@ -7728,7 +7814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:85">
+    <row r="58" spans="1:85" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>0</v>
       </c>
@@ -7847,7 +7933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:85">
+    <row r="59" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0</v>
       </c>
@@ -7975,7 +8061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:85">
+    <row r="60" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -8103,7 +8189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:85">
+    <row r="61" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2</v>
       </c>
@@ -8231,7 +8317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:85">
+    <row r="62" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3</v>
       </c>
@@ -8359,7 +8445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:85">
+    <row r="63" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>4</v>
       </c>
@@ -8487,7 +8573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:85">
+    <row r="64" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>5</v>
       </c>
@@ -8615,7 +8701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:72">
+    <row r="65" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>6</v>
       </c>
@@ -8743,7 +8829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:72">
+    <row r="66" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>7</v>
       </c>
@@ -8871,7 +8957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:72">
+    <row r="67" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>8</v>
       </c>
@@ -8999,7 +9085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:72">
+    <row r="68" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9</v>
       </c>
@@ -9127,7 +9213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:72">
+    <row r="69" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>10</v>
       </c>
@@ -9255,7 +9341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:72">
+    <row r="70" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>11</v>
       </c>
@@ -9383,7 +9469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:72">
+    <row r="71" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>12</v>
       </c>
@@ -9511,7 +9597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:72">
+    <row r="72" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>13</v>
       </c>
@@ -9639,7 +9725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:72">
+    <row r="73" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>14</v>
       </c>
@@ -9767,7 +9853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:72">
+    <row r="74" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>15</v>
       </c>
@@ -9903,24 +9989,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the robotron ply file thingy to keep the bounding boxes. Generated a bunch of robotron ply files.
</commit_message>
<xml_diff>
--- a/6044_FramPat/SAM/Robotron 2084/Sprite map/sprite - Brain.xlsx
+++ b/6044_FramPat/SAM/Robotron 2084/Sprite map/sprite - Brain.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097F38C4-1F2F-4C7B-91CC-04191A1E2657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2526" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2538" uniqueCount="32">
   <si>
     <t>B</t>
   </si>
@@ -78,12 +77,48 @@
   <si>
     <t>g</t>
   </si>
+  <si>
+    <t>brain1</t>
+  </si>
+  <si>
+    <t>brain2</t>
+  </si>
+  <si>
+    <t>brain3</t>
+  </si>
+  <si>
+    <t>brain5</t>
+  </si>
+  <si>
+    <t>brain4</t>
+  </si>
+  <si>
+    <t>brain6</t>
+  </si>
+  <si>
+    <t>brain7</t>
+  </si>
+  <si>
+    <t>brain8</t>
+  </si>
+  <si>
+    <t>brain9</t>
+  </si>
+  <si>
+    <t>brain10</t>
+  </si>
+  <si>
+    <t>brain11</t>
+  </si>
+  <si>
+    <t>brain12</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,7 +309,7 @@
         <xdr:cNvPr id="1028" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -320,7 +355,7 @@
         <xdr:cNvPr id="2" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -366,7 +401,7 @@
         <xdr:cNvPr id="3" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -412,7 +447,7 @@
         <xdr:cNvPr id="4" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -458,7 +493,7 @@
         <xdr:cNvPr id="5" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -504,7 +539,7 @@
         <xdr:cNvPr id="6" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -550,7 +585,7 @@
         <xdr:cNvPr id="7" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -581,22 +616,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>131381</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>39414</xdr:rowOff>
+      <xdr:colOff>124812</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>183931</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
-      <xdr:colOff>102806</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>29889</xdr:rowOff>
+      <xdr:colOff>96237</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>174406</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="8" name="Picture 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -613,7 +648,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8322881" y="7468914"/>
+          <a:off x="8316312" y="7422931"/>
           <a:ext cx="2447925" cy="3038475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -642,7 +677,7 @@
         <xdr:cNvPr id="9" name="Picture 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -688,7 +723,7 @@
         <xdr:cNvPr id="10" name="Picture 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -734,7 +769,7 @@
         <xdr:cNvPr id="11" name="Picture 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -780,7 +815,7 @@
         <xdr:cNvPr id="12" name="Picture 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -812,9 +847,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -852,7 +887,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -886,7 +921,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -921,10 +955,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1097,19 +1130,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CL74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:CL75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="CL8" sqref="CL8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="BT74" sqref="BH59:BT74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="98" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:88">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -1228,7 +1261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:88">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1362,7 +1395,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:88">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1496,7 +1529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:88">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1630,7 +1663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:88">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1764,7 +1797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:88">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1898,7 +1931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:88">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2032,7 +2065,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:88">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2166,7 +2199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:88">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2300,7 +2333,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:88">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2434,7 +2467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:88">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2568,7 +2601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:88">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2696,7 +2729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:88">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2824,7 +2857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:88">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2952,7 +2985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:88">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3080,7 +3113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:88">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3208,7 +3241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:90">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3251,6 +3284,9 @@
       <c r="N17" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="R17" t="s">
+        <v>20</v>
+      </c>
       <c r="AD17">
         <v>15</v>
       </c>
@@ -3293,6 +3329,9 @@
       <c r="AQ17" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="AU17" t="s">
+        <v>21</v>
+      </c>
       <c r="BG17">
         <v>15</v>
       </c>
@@ -3335,8 +3374,11 @@
       <c r="BT17" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="BW17" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="20" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:90">
       <c r="B20" s="1">
         <v>0</v>
       </c>
@@ -3460,7 +3502,7 @@
       <c r="CK20" s="1"/>
       <c r="CL20" s="1"/>
     </row>
-    <row r="21" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:90">
       <c r="A21">
         <v>0</v>
       </c>
@@ -3588,7 +3630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:90">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3716,7 +3758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:90">
       <c r="A23">
         <v>2</v>
       </c>
@@ -3844,7 +3886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:90">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3972,7 +4014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:90">
       <c r="A25">
         <v>4</v>
       </c>
@@ -4100,7 +4142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:90">
       <c r="A26">
         <v>5</v>
       </c>
@@ -4228,7 +4270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:90">
       <c r="A27">
         <v>6</v>
       </c>
@@ -4356,7 +4398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:90">
       <c r="A28">
         <v>7</v>
       </c>
@@ -4484,7 +4526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:90">
       <c r="A29">
         <v>8</v>
       </c>
@@ -4615,7 +4657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:90">
       <c r="A30">
         <v>9</v>
       </c>
@@ -4746,7 +4788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:90">
       <c r="A31">
         <v>10</v>
       </c>
@@ -4877,7 +4919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:90">
       <c r="A32">
         <v>11</v>
       </c>
@@ -5008,7 +5050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:75">
       <c r="A33">
         <v>12</v>
       </c>
@@ -5139,7 +5181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:75">
       <c r="A34">
         <v>13</v>
       </c>
@@ -5270,7 +5312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:75">
       <c r="A35">
         <v>14</v>
       </c>
@@ -5401,7 +5443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:75">
       <c r="A36">
         <v>15</v>
       </c>
@@ -5532,17 +5574,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:75">
+      <c r="Q37" t="s">
+        <v>24</v>
+      </c>
       <c r="AB37" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="AU37" t="s">
+        <v>23</v>
+      </c>
+      <c r="BW37" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="38" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:75">
       <c r="AB38" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:75">
       <c r="B39" s="1">
         <v>0</v>
       </c>
@@ -5661,7 +5712,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:75">
       <c r="A40">
         <v>0</v>
       </c>
@@ -5794,7 +5845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:75">
       <c r="A41">
         <v>1</v>
       </c>
@@ -5927,7 +5978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:75">
       <c r="A42">
         <v>2</v>
       </c>
@@ -6060,7 +6111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:75">
       <c r="A43">
         <v>3</v>
       </c>
@@ -6193,7 +6244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:75">
       <c r="A44">
         <v>4</v>
       </c>
@@ -6326,7 +6377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:75">
       <c r="A45">
         <v>5</v>
       </c>
@@ -6459,7 +6510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:75">
       <c r="A46">
         <v>6</v>
       </c>
@@ -6592,7 +6643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:75">
       <c r="A47">
         <v>7</v>
       </c>
@@ -6725,7 +6776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:75">
       <c r="A48">
         <v>8</v>
       </c>
@@ -6858,7 +6909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:85">
       <c r="A49">
         <v>9</v>
       </c>
@@ -6991,7 +7042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:85">
       <c r="A50">
         <v>10</v>
       </c>
@@ -7154,7 +7205,7 @@
       <c r="CF50" s="1"/>
       <c r="CG50" s="1"/>
     </row>
-    <row r="51" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:85">
       <c r="A51">
         <v>11</v>
       </c>
@@ -7286,7 +7337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:85">
       <c r="A52">
         <v>12</v>
       </c>
@@ -7418,7 +7469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:85">
       <c r="A53">
         <v>13</v>
       </c>
@@ -7550,7 +7601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:85">
       <c r="A54">
         <v>14</v>
       </c>
@@ -7682,7 +7733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:85">
       <c r="A55">
         <v>15</v>
       </c>
@@ -7814,7 +7865,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:85">
+      <c r="R56" t="s">
+        <v>26</v>
+      </c>
+      <c r="AT56" t="s">
+        <v>27</v>
+      </c>
+      <c r="BW56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:85">
       <c r="B58" s="1">
         <v>0</v>
       </c>
@@ -7933,7 +7995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:85">
       <c r="A59">
         <v>0</v>
       </c>
@@ -8061,7 +8123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:85">
       <c r="A60">
         <v>1</v>
       </c>
@@ -8189,7 +8251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:85">
       <c r="A61">
         <v>2</v>
       </c>
@@ -8317,7 +8379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:85">
       <c r="A62">
         <v>3</v>
       </c>
@@ -8445,7 +8507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:85">
       <c r="A63">
         <v>4</v>
       </c>
@@ -8573,7 +8635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:85">
       <c r="A64">
         <v>5</v>
       </c>
@@ -8701,7 +8763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:76">
       <c r="A65">
         <v>6</v>
       </c>
@@ -8829,7 +8891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:76">
       <c r="A66">
         <v>7</v>
       </c>
@@ -8957,7 +9019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:76">
       <c r="A67">
         <v>8</v>
       </c>
@@ -9085,7 +9147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:76">
       <c r="A68">
         <v>9</v>
       </c>
@@ -9213,7 +9275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:76">
       <c r="A69">
         <v>10</v>
       </c>
@@ -9341,7 +9403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:76">
       <c r="A70">
         <v>11</v>
       </c>
@@ -9469,7 +9531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:76">
       <c r="A71">
         <v>12</v>
       </c>
@@ -9597,7 +9659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:76">
       <c r="A72">
         <v>13</v>
       </c>
@@ -9725,7 +9787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:76">
       <c r="A73">
         <v>14</v>
       </c>
@@ -9853,7 +9915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:76">
       <c r="A74">
         <v>15</v>
       </c>
@@ -9979,6 +10041,17 @@
       </c>
       <c r="BT74" s="4" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:76">
+      <c r="R75" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU75" t="s">
+        <v>30</v>
+      </c>
+      <c r="BX75" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -9989,24 +10062,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>